<commit_message>
added vline to graphs
</commit_message>
<xml_diff>
--- a/part2/data/restrictions.xlsx
+++ b/part2/data/restrictions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alechay/r_projects/GitHub/covid19-rt/part2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5BB87C2-796E-7641-B300-306FE6A9D59F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3329D85D-6635-9D4B-A2CF-4021AB235553}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15320" yWindow="2480" windowWidth="16640" windowHeight="17440" xr2:uid="{19028CAC-2451-E34D-A1CB-F4A95A37F047}"/>
+    <workbookView xWindow="15860" yWindow="620" windowWidth="16640" windowHeight="17440" xr2:uid="{19028CAC-2451-E34D-A1CB-F4A95A37F047}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="12">
   <si>
     <t>Toronto</t>
   </si>
@@ -51,25 +51,25 @@
     <t>Halton</t>
   </si>
   <si>
-    <t>Lockdown</t>
-  </si>
-  <si>
     <t>Date_start</t>
   </si>
   <si>
     <t>Date_end</t>
   </si>
   <si>
-    <t>Gathering limits</t>
-  </si>
-  <si>
-    <t>Stage 1/Red</t>
-  </si>
-  <si>
-    <t>Stage 3/ Yellow</t>
-  </si>
-  <si>
-    <t>Stage 2/Modified Stage 2/Orange</t>
+    <t>Enhanced lockdown</t>
+  </si>
+  <si>
+    <t>Lockdown/Stage 1</t>
+  </si>
+  <si>
+    <t>Red/Stage 2/Modified Stage 2</t>
+  </si>
+  <si>
+    <t>Orange/Gathering limits</t>
+  </si>
+  <si>
+    <t>Green/Stage 3</t>
   </si>
 </sst>
 </file>
@@ -85,42 +85,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -135,14 +105,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,20 +422,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5E87830-58E6-7B4A-BE0D-BA708A599FE5}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -490,394 +455,420 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
+        <v>43876</v>
+      </c>
+      <c r="B2" s="1">
         <v>43907</v>
       </c>
-      <c r="B2" s="1">
-        <v>43970</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>5</v>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
+        <v>43907</v>
+      </c>
+      <c r="B3" s="1">
         <v>43970</v>
       </c>
-      <c r="B3" s="1">
-        <v>44001</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>9</v>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
+        <v>43970</v>
+      </c>
+      <c r="B4" s="1">
         <v>44001</v>
       </c>
-      <c r="B4" s="1">
-        <v>44006</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>11</v>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
+        <v>44001</v>
+      </c>
+      <c r="B5" s="1">
         <v>44006</v>
       </c>
-      <c r="B5" s="1">
-        <v>44036</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>11</v>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
+        <v>44006</v>
+      </c>
+      <c r="B6" s="1">
         <v>44036</v>
       </c>
-      <c r="B6" s="1">
-        <v>44043</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>10</v>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
+        <v>44036</v>
+      </c>
+      <c r="B7" s="1">
         <v>44043</v>
       </c>
-      <c r="B7" s="1">
-        <v>44092</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>10</v>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
+        <v>44043</v>
+      </c>
+      <c r="B8" s="1">
         <v>44092</v>
       </c>
-      <c r="B8" s="1">
-        <v>44114</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>10</v>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
+        <v>44092</v>
+      </c>
+      <c r="B9" s="1">
         <v>44114</v>
       </c>
-      <c r="B9" s="1">
-        <v>44123</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="5" t="s">
+      <c r="C9" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="D9" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>10</v>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
+        <v>44114</v>
+      </c>
+      <c r="B10" s="1">
         <v>44123</v>
       </c>
-      <c r="B10" s="1">
-        <v>44142</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>10</v>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
+        <v>44123</v>
+      </c>
+      <c r="B11" s="1">
         <v>44142</v>
       </c>
-      <c r="B11" s="1">
-        <v>44151</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>10</v>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
+        <v>44142</v>
+      </c>
+      <c r="B12" s="1">
         <v>44151</v>
       </c>
-      <c r="B12" s="1">
-        <v>44158</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="4" t="s">
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
+        <v>44151</v>
+      </c>
+      <c r="B13" s="1">
         <v>44158</v>
       </c>
-      <c r="B13" s="1">
-        <v>44179</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>11</v>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
+        <v>44158</v>
+      </c>
+      <c r="B14" s="1">
         <v>44179</v>
       </c>
-      <c r="B14" s="1">
-        <v>44191</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>11</v>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
+        <v>44179</v>
+      </c>
+      <c r="B15" s="1">
         <v>44191</v>
       </c>
-      <c r="B15" s="1">
-        <v>44243</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>5</v>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
+        <v>44191</v>
+      </c>
+      <c r="B16" s="1">
         <v>44243</v>
       </c>
-      <c r="B16" s="1">
-        <v>44249</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>11</v>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
+        <v>44243</v>
+      </c>
+      <c r="B17" s="1">
         <v>44249</v>
       </c>
-      <c r="B17" s="1">
-        <v>44274</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>11</v>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
+        <v>44249</v>
+      </c>
+      <c r="B18" s="1">
         <v>44274</v>
       </c>
-      <c r="B18" s="1">
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>44274</v>
+      </c>
+      <c r="B19" s="1">
         <v>44286</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>